<commit_message>
feat - formatting field
</commit_message>
<xml_diff>
--- a/output/changelog.xlsx
+++ b/output/changelog.xlsx
@@ -16,7 +16,7 @@
     <t>ENDPOINT</t>
   </si>
   <si>
-    <t>PATH</t>
+    <t>CAMINHO</t>
   </si>
   <si>
     <t>CAMPO</t>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>info</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>description</t>
@@ -97,6 +94,9 @@
 '</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>version</t>
   </si>
   <si>
@@ -115,67 +115,67 @@
     <t>contracts/</t>
   </si>
   <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>Campo 'pattern' alterado de '^[a-zA-Z0-9][a-zA-Z0-9\-]{0,99}$' para '^[a-zA-Z0-9][a-zA-Z0-9-]{0,99}$'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/contractId</t>
   </si>
   <si>
-    <t>pattern</t>
-  </si>
-  <si>
-    <t>Campo 'pattern' alterado de '^[a-zA-Z0-9][a-zA-Z0-9\-]{0,99}$' para '^[a-zA-Z0-9][a-zA-Z0-9-]{0,99}$'</t>
-  </si>
-  <si>
     <t>minLength</t>
   </si>
   <si>
     <t>Campo 'minLength' adicionado.</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/items/properties/brandName</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Nome da Marca reportada pelo participante do Open Banking. O conceito a que se refere a 'marca' é em essência uma promessa da empresa em fornecer uma série específica de atributos, benefícios e serviços uniformes aos clientes' para 'Nome da Marca reportada pelo participante no Open Finance. Recomenda-se utilizar, sempre que possível, o mesmo nome de marca atribuído no campo do diretório Customer Friendly Server Name (Authorisation Server).
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/items/properties/brandName</t>
+  </si>
+  <si>
+    <t>Campo 'pattern' alterado de '\d{14}|^NA$' para '^\d{14}$'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/companyCnpj</t>
   </si>
   <si>
-    <t>Campo 'pattern' alterado de '\d{14}|^NA$' para '^\d{14}$'</t>
+    <t>maxLength</t>
+  </si>
+  <si>
+    <t>Campo 'maxLength' removido.</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/productType</t>
   </si>
   <si>
-    <t>maxLength</t>
-  </si>
-  <si>
-    <t>Campo 'maxLength' removido.</t>
-  </si>
-  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/ipocCode</t>
   </si>
   <si>
     <t>Campo 'pattern' adicionado.</t>
   </si>
   <si>
+    <t>additionalProperties</t>
+  </si>
+  <si>
+    <t>Campo 'additionalProperties' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items</t>
   </si>
   <si>
-    <t>additionalProperties</t>
-  </si>
-  <si>
-    <t>Campo 'additionalProperties' removido.</t>
+    <t>minItems</t>
+  </si>
+  <si>
+    <t>Campo 'minItems' alterado de '1' para '0'</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data</t>
   </si>
   <si>
-    <t>minItems</t>
-  </si>
-  <si>
-    <t>Campo 'minItems' alterado de '1' para '0'</t>
-  </si>
-  <si>
     <t>get/responses/200/content/application/json/schema/properties/links</t>
   </si>
   <si>
@@ -257,42 +257,42 @@
     <t>get/responses/500/content/application/json; charset=utf-8/schema</t>
   </si>
   <si>
+    <t>Campo 'description' alterado de 'Lista de contratos obtida com sucesso.' para 'Erro inesperado.'</t>
+  </si>
+  <si>
     <t>get/responses/default</t>
   </si>
   <si>
-    <t>Campo 'description' alterado de 'Lista de contratos obtida com sucesso.' para 'Erro inesperado.'</t>
-  </si>
-  <si>
     <t>headers</t>
   </si>
   <si>
     <t>Campo 'headers' removido.</t>
   </si>
   <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>Campo 'application/json' removido.</t>
+  </si>
+  <si>
     <t>get/responses/default/content</t>
   </si>
   <si>
-    <t>application/json</t>
-  </si>
-  <si>
-    <t>Campo 'application/json' removido.</t>
-  </si>
-  <si>
     <t>application/json; charset=utf-8</t>
   </si>
   <si>
     <t>Campo 'application/json; charset=utf-8' adicionado.</t>
   </si>
   <si>
+    <t>422</t>
+  </si>
+  <si>
+    <t>Campo '422' adicionado.</t>
+  </si>
+  <si>
     <t>get/responses</t>
   </si>
   <si>
-    <t>422</t>
-  </si>
-  <si>
-    <t>Campo '422' adicionado.</t>
-  </si>
-  <si>
     <t>423</t>
   </si>
   <si>
@@ -308,15 +308,15 @@
     <t>contracts/{contractId}/</t>
   </si>
   <si>
+    <t>contractAmount</t>
+  </si>
+  <si>
+    <t>Campo 'contractAmount' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/required</t>
   </si>
   <si>
-    <t>contractAmount</t>
-  </si>
-  <si>
-    <t>Campo 'contractAmount' removido.</t>
-  </si>
-  <si>
     <t>settlementDate</t>
   </si>
   <si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractNumber</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/ipocCode</t>
   </si>
   <si>
     <t>Campo 'description' alterado de '"Número padronizado do contrato - IPOC (Identificação Padronizada da Operação de Crédito). Segundo DOC 3040, composta por:
@@ -374,7 +371,7 @@
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/productName</t>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/ipocCode</t>
   </si>
   <si>
     <t>Campo 'description' alterado de '"Denominação/Identificação do nome da Modalidade da Operação de Crédito divulgado ao cliente"
@@ -382,28 +379,31 @@
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/productName</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/productType</t>
   </si>
   <si>
+    <t>disbursementDate</t>
+  </si>
+  <si>
+    <t>Campo 'disbursementDate' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties</t>
   </si>
   <si>
-    <t>disbursementDate</t>
-  </si>
-  <si>
-    <t>Campo 'disbursementDate' removido.</t>
-  </si>
-  <si>
     <t>disbursementDates</t>
   </si>
   <si>
     <t>Campo 'disbursementDates' adicionado.</t>
   </si>
   <si>
+    <t>Campo 'pattern' alterado de '^(\d{4})-(1[0-2]|0?[1-9])-(3[01]|[12][0-9]|0?[1-9])$|^NA$' para '^(\d{4})-(1[0-2]|0?[1-9])-(3[01]|[12][0-9]|0?[1-9])$'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/settlementDate</t>
-  </si>
-  <si>
-    <t>Campo 'pattern' alterado de '^(\d{4})-(1[0-2]|0?[1-9])-(3[01]|[12][0-9]|0?[1-9])$|^NA$' para '^(\d{4})-(1[0-2]|0?[1-9])-(3[01]|[12][0-9]|0?[1-9])$'</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Data de liquidação da operação.
@@ -412,12 +412,12 @@
 '</t>
   </si>
   <si>
+    <t>Campo 'description' alterado de 'Valor contratado da operação. Expresso em valor monetário com até 4 casas decimais' para 'Valor contratado da operação. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractAmount</t>
   </si>
   <si>
-    <t>Campo 'description' alterado de 'Valor contratado da operação. Expresso em valor monetário com até 4 casas decimais' para 'Valor contratado da operação. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -446,9 +446,6 @@
   </si>
   <si>
     <t>Campo 'nullable' removido.</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/currency</t>
   </si>
   <si>
     <t>Campo 'description' alterado de '"Moeda referente ao valor da garantia, segundo modelo ISO-4217. p.ex. 'BRL'
@@ -458,17 +455,17 @@
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/dueDate</t>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/currency</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Data de vencimento Final da operação. Especificação RFC-3339' para 'Data de vencimento Final da operação. Especificação RFC-3339
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/dueDate</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/instalmentPeriodicity</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/instalmentPeriodicityAdditionalInfo</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Campo obrigatório para complementar a informação relativa à periodicidade de pagamento regular quando tiver a opção OUTROS.
@@ -477,11 +474,14 @@
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/firstInstalmentDueDate</t>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/instalmentPeriodicityAdditionalInfo</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Data de vencimento primeira parcela do principal' para 'Data de vencimento primeira parcela do principal
 '</t>
+  </si>
+  <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/firstInstalmentDueDate</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/CET</t>
@@ -507,10 +507,10 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/amortizationScheduled</t>
   </si>
   <si>
+    <t>Campo 'maxLength' alterado de '50' para '200'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/amortizationScheduledAdditionalInfo</t>
-  </si>
-  <si>
-    <t>Campo 'maxLength' alterado de '50' para '200'</t>
   </si>
   <si>
     <t>Campo 'example' alterado de 'NA' para 'Informações complementares relativa à amortização do tipo 'OUTROS''</t>
@@ -522,13 +522,13 @@
 '</t>
   </si>
   <si>
+    <t>additionalInfo</t>
+  </si>
+  <si>
+    <t>Campo 'additionalInfo' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates/items/required</t>
-  </si>
-  <si>
-    <t>additionalInfo</t>
-  </si>
-  <si>
-    <t>Campo 'additionalInfo' removido.</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates/items/properties/taxType</t>
@@ -577,33 +577,33 @@
     <t>Campo 'example' alterado de '0.55' para '0.550000'</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates/items/properties/additionalInfo</t>
-  </si>
-  <si>
     <t>Campo 'description' alterado de 'Texto com informações adicionais sobre a composição das taxas de juros pactuadas' para 'Texto com informações adicionais sobre a composição das taxas de juros pactuadas. 
 [Restrição] Caso a instituição possua a informação para compartilhamento, esta deverá ser informada.
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates/items/properties/additionalInfo</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates/items</t>
   </si>
   <si>
+    <t>Campo 'minItems' adicionado.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/interestRates</t>
   </si>
   <si>
-    <t>Campo 'minItems' adicionado.</t>
-  </si>
-  <si>
     <t>Campo 'description' adicionado.</t>
   </si>
   <si>
+    <t>feeAmount</t>
+  </si>
+  <si>
+    <t>Campo 'feeAmount' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFees/items/required</t>
-  </si>
-  <si>
-    <t>feeAmount</t>
-  </si>
-  <si>
-    <t>Campo 'feeAmount' removido.</t>
   </si>
   <si>
     <t>feeRate</t>
@@ -649,25 +649,22 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFees/items</t>
   </si>
   <si>
+    <t>Campo 'description' alterado de 'Lista que traz a relação de tarifas pactuadas no contrato' para 'Lista que traz o conjunto de informações necessárias para demonstrar a composição das taxas de juros remuneratórios da Modalidade de crédito'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFees</t>
   </si>
   <si>
-    <t>Campo 'description' alterado de 'Lista que traz a relação de tarifas pactuadas no contrato' para 'Lista que traz o conjunto de informações necessárias para demonstrar a composição das taxas de juros remuneratórios da Modalidade de crédito'</t>
+    <t>chargeAdditionalInfo</t>
+  </si>
+  <si>
+    <t>Campo 'chargeAdditionalInfo' removido.</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFinanceCharges/items/required</t>
   </si>
   <si>
-    <t>chargeAdditionalInfo</t>
-  </si>
-  <si>
-    <t>Campo 'chargeAdditionalInfo' removido.</t>
-  </si>
-  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFinanceCharges/items/properties/chargeType</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFinanceCharges/items/properties/chargeAdditionalInfo</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Campo para informações adicionais.
@@ -677,6 +674,9 @@
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFinanceCharges/items/properties/chargeAdditionalInfo</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractedFinanceCharges/items/properties/chargeRate</t>
   </si>
   <si>
@@ -710,27 +710,27 @@
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantyType</t>
   </si>
   <si>
+    <t>SEM_TIPO_GARANTIA</t>
+  </si>
+  <si>
+    <t>Campo 'SEM_TIPO_GARANTIA' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantyType/enum</t>
   </si>
   <si>
-    <t>SEM_TIPO_GARANTIA</t>
-  </si>
-  <si>
-    <t>Campo 'SEM_TIPO_GARANTIA' removido.</t>
-  </si>
-  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantySubType</t>
   </si>
   <si>
+    <t>ACORDOS_COMPENSACAO_LIQUIDACAO_OBRIGACOES</t>
+  </si>
+  <si>
+    <t>Campo 'ACORDOS_COMPENSACAO_LIQUIDACAO_OBRIGACOES' adicionado.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantySubType/enum</t>
   </si>
   <si>
-    <t>ACORDOS_COMPENSACAO_LIQUIDACAO_OBRIGACOES</t>
-  </si>
-  <si>
-    <t>Campo 'ACORDOS_COMPENSACAO_LIQUIDACAO_OBRIGACOES' adicionado.</t>
-  </si>
-  <si>
     <t>PROAGRO</t>
   </si>
   <si>
@@ -741,9 +741,6 @@
   </si>
   <si>
     <t>Campo 'SEM_SUB_TIPO_GARANTIA' adicionado.</t>
-  </si>
-  <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantyAmount</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Valor original da garantia. Valor monetário, expresso com até 4 casas decimais.
@@ -751,6 +748,9 @@
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/items/properties/warrantyAmount</t>
+  </si>
+  <si>
     <t>Campo 'description' alterado de 'Lista de garantias vinculadas ao contrato de adiantamento a depositantes identificado por contractId' para 'Erro inesperado.'</t>
   </si>
   <si>
@@ -821,12 +821,12 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/balloonPayments/items/properties</t>
   </si>
   <si>
+    <t>Campo 'description' alterado de 'Valor monetário da parcela não regular a vencer. Expresso em valor monetário com 4 casas decimais.' para 'Valor monetário da parcela não regular a vencer. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/balloonPayments/items/properties/amount</t>
   </si>
   <si>
-    <t>Campo 'description' alterado de 'Valor monetário da parcela não regular a vencer. Expresso em valor monetário com 4 casas decimais.' para 'Valor monetário da parcela não regular a vencer. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
-  </si>
-  <si>
     <t>Campo 'type' alterado de 'number' para 'object'</t>
   </si>
   <si>
@@ -854,12 +854,12 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/balloonPayments/items</t>
   </si>
   <si>
+    <t>Campo 'minItems' alterado de '0' para '1'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/balloonPayments</t>
   </si>
   <si>
-    <t>Campo 'minItems' alterado de '0' para '1'</t>
-  </si>
-  <si>
     <t>Campo 'description' alterado de 'Dados do cronograma de parcelas do contrato de adiantamento a depositantes identificado por contractId' para 'Erro inesperado.'</t>
   </si>
   <si>
@@ -875,13 +875,13 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/contractOutstandingBalance</t>
   </si>
   <si>
+    <t>overParcel</t>
+  </si>
+  <si>
+    <t>Campo 'overParcel' removido.</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/required</t>
-  </si>
-  <si>
-    <t>overParcel</t>
-  </si>
-  <si>
-    <t>Campo 'overParcel' removido.</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/paymentId</t>
@@ -900,26 +900,26 @@
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel</t>
-  </si>
-  <si>
     <t>Campo 'description' alterado de 'Objeto das tarifas e encargos que foram pagos fora da parcela.' para 'Objeto das tarifas e encargos que foram pagos fora da parcela.
 [Restrição] Informação deve ser enviada caso ela exista, torna-se obrigatório caso haja parcelamento.
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/fees/items/properties/feeName</t>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Denominação da Tarifa pactuada' para 'Denominação da Tarifa pactuada.
 '</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/fees/items/properties/feeCode</t>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/fees/items/properties/feeName</t>
   </si>
   <si>
     <t>Campo 'description' alterado de 'Sigla identificadora da tarifa avulsa fora da parcela' para 'Sigla identificadora da tarifa pactuada.
 '</t>
+  </si>
+  <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/fees/items/properties/feeCode</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/fees/items/properties/feeAmount</t>
@@ -944,9 +944,6 @@
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/charges/items/properties/chargeType</t>
   </si>
   <si>
-    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/charges/items/properties/chargeAdditionalInfo</t>
-  </si>
-  <si>
     <t>Campo 'description' alterado de 'Campo livre para preenchimento das informações adicionais referente ao encargo.
 [Restrição] Obrigatório quando chargeType for igual OUTROS.
 ' para 'Campo livre para preenchimento das informações adicionais referente ao encargo.
@@ -954,10 +951,13 @@
 '</t>
   </si>
   <si>
+    <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/charges/items/properties/chargeAdditionalInfo</t>
+  </si>
+  <si>
+    <t>Campo 'description' alterado de 'Valor do pagamento do encargo pago fora da parcela. Expresso em valor monetário com até 4 casas decimais.' para 'Valor do pagamento do encargo pago fora da parcela. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
+  </si>
+  <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/charges/items/properties/chargeAmount</t>
-  </si>
-  <si>
-    <t>Campo 'description' alterado de 'Valor do pagamento do encargo pago fora da parcela. Expresso em valor monetário com até 4 casas decimais.' para 'Valor do pagamento do encargo pago fora da parcela. Expresso em valor monetário com no mínimo 2 casas e no máximo 4 casas decimais.'</t>
   </si>
   <si>
     <t>get/responses/200/content/application/json/schema/properties/data/properties/releases/items/properties/overParcel/properties/charges/items</t>
@@ -1037,13 +1037,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1051,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
@@ -1065,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -1079,13 +1079,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1093,7 +1093,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>17</v>
@@ -1107,13 +1107,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1121,13 +1121,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1135,13 +1135,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1166,7 +1166,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>27</v>
@@ -1177,13 +1177,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1191,13 +1191,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1208,10 +1208,10 @@
         <v>34</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1222,10 +1222,10 @@
         <v>35</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1236,10 +1236,10 @@
         <v>36</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1250,10 +1250,10 @@
         <v>37</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1264,10 +1264,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1278,10 +1278,10 @@
         <v>39</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1292,10 +1292,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1306,10 +1306,10 @@
         <v>41</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1320,10 +1320,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1334,10 +1334,10 @@
         <v>43</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1348,10 +1348,10 @@
         <v>44</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1362,10 +1362,10 @@
         <v>45</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1376,10 +1376,10 @@
         <v>46</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1390,10 +1390,10 @@
         <v>47</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1404,10 +1404,10 @@
         <v>48</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1418,10 +1418,10 @@
         <v>49</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1432,10 +1432,10 @@
         <v>50</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1446,10 +1446,10 @@
         <v>51</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1460,10 +1460,10 @@
         <v>52</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1474,10 +1474,10 @@
         <v>53</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1488,10 +1488,10 @@
         <v>54</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1502,10 +1502,10 @@
         <v>55</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1516,10 +1516,10 @@
         <v>56</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1530,10 +1530,10 @@
         <v>57</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1544,10 +1544,10 @@
         <v>58</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1558,10 +1558,10 @@
         <v>59</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1572,10 +1572,10 @@
         <v>60</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1583,13 +1583,13 @@
         <v>13</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1597,7 +1597,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>63</v>
@@ -1611,13 +1611,13 @@
         <v>13</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="D43" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1625,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>68</v>
@@ -1639,13 +1639,13 @@
         <v>13</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="D45" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1653,7 +1653,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>73</v>
@@ -1667,7 +1667,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>75</v>
@@ -1681,13 +1681,13 @@
         <v>77</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="D48" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1695,7 +1695,7 @@
         <v>77</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>81</v>
@@ -1709,7 +1709,7 @@
         <v>77</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>83</v>
@@ -1723,7 +1723,7 @@
         <v>77</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>85</v>
@@ -1737,7 +1737,7 @@
         <v>77</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>87</v>
@@ -1751,7 +1751,7 @@
         <v>77</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>89</v>
@@ -1782,7 +1782,7 @@
         <v>91</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>27</v>
@@ -1793,13 +1793,13 @@
         <v>77</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1807,7 +1807,7 @@
         <v>77</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>17</v>
@@ -1821,10 +1821,10 @@
         <v>77</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>27</v>
@@ -1835,13 +1835,13 @@
         <v>77</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1852,10 +1852,10 @@
         <v>96</v>
       </c>
       <c r="C60" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1863,13 +1863,13 @@
         <v>77</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="D61" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1877,7 +1877,7 @@
         <v>77</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>100</v>
@@ -1891,13 +1891,13 @@
         <v>77</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1905,10 +1905,10 @@
         <v>77</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>104</v>
@@ -1919,13 +1919,13 @@
         <v>77</v>
       </c>
       <c r="B65" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1933,7 +1933,7 @@
         <v>77</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>107</v>
@@ -1947,7 +1947,7 @@
         <v>77</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>109</v>
@@ -1961,10 +1961,10 @@
         <v>77</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>111</v>
@@ -1975,7 +1975,7 @@
         <v>77</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>17</v>
@@ -1989,7 +1989,7 @@
         <v>77</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>113</v>
@@ -2003,7 +2003,7 @@
         <v>77</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>115</v>
@@ -2017,13 +2017,13 @@
         <v>77</v>
       </c>
       <c r="B72" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2031,13 +2031,13 @@
         <v>77</v>
       </c>
       <c r="B73" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2045,7 +2045,7 @@
         <v>77</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>17</v>
@@ -2062,10 +2062,10 @@
         <v>121</v>
       </c>
       <c r="C75" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2073,13 +2073,13 @@
         <v>77</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2087,13 +2087,13 @@
         <v>77</v>
       </c>
       <c r="B77" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2101,7 +2101,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>17</v>
@@ -2132,7 +2132,7 @@
         <v>126</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>127</v>
@@ -2146,7 +2146,7 @@
         <v>126</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>128</v>
@@ -2188,7 +2188,7 @@
         <v>126</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>27</v>
@@ -2230,10 +2230,10 @@
         <v>131</v>
       </c>
       <c r="C87" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2241,13 +2241,13 @@
         <v>77</v>
       </c>
       <c r="B88" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2255,7 +2255,7 @@
         <v>77</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>113</v>
@@ -2269,10 +2269,10 @@
         <v>77</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>135</v>
@@ -2283,13 +2283,13 @@
         <v>77</v>
       </c>
       <c r="B91" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="D91" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2300,10 +2300,10 @@
         <v>139</v>
       </c>
       <c r="C92" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D92" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2314,10 +2314,10 @@
         <v>140</v>
       </c>
       <c r="C93" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2328,10 +2328,10 @@
         <v>141</v>
       </c>
       <c r="C94" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2342,10 +2342,10 @@
         <v>142</v>
       </c>
       <c r="C95" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2356,10 +2356,10 @@
         <v>143</v>
       </c>
       <c r="C96" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2370,10 +2370,10 @@
         <v>144</v>
       </c>
       <c r="C97" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2398,7 +2398,7 @@
         <v>145</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>146</v>
@@ -2412,7 +2412,7 @@
         <v>145</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>128</v>
@@ -2468,7 +2468,7 @@
         <v>145</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>27</v>
@@ -2510,7 +2510,7 @@
         <v>148</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>149</v>
@@ -2524,7 +2524,7 @@
         <v>148</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>128</v>
@@ -2566,7 +2566,7 @@
         <v>148</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>27</v>
@@ -2591,13 +2591,13 @@
         <v>77</v>
       </c>
       <c r="B113" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2608,10 +2608,10 @@
         <v>153</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2619,13 +2619,13 @@
         <v>77</v>
       </c>
       <c r="B115" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D115" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C115" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2633,10 +2633,10 @@
         <v>77</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>156</v>
@@ -2647,13 +2647,13 @@
         <v>77</v>
       </c>
       <c r="B117" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C117" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C117" s="0" t="s">
+      <c r="D117" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2661,7 +2661,7 @@
         <v>77</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>160</v>
@@ -2678,10 +2678,10 @@
         <v>162</v>
       </c>
       <c r="C119" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2692,10 +2692,10 @@
         <v>163</v>
       </c>
       <c r="C120" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D120" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2720,7 +2720,7 @@
         <v>164</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>165</v>
@@ -2734,7 +2734,7 @@
         <v>164</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>166</v>
@@ -2804,7 +2804,7 @@
         <v>168</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>169</v>
@@ -2818,7 +2818,7 @@
         <v>168</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>128</v>
@@ -2860,7 +2860,7 @@
         <v>168</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>27</v>
@@ -2888,10 +2888,10 @@
         <v>171</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2899,13 +2899,13 @@
         <v>77</v>
       </c>
       <c r="B135" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D135" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D135" s="0" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2913,13 +2913,13 @@
         <v>77</v>
       </c>
       <c r="B136" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C136" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C136" s="0" t="s">
+      <c r="D136" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D136" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2930,10 +2930,10 @@
         <v>177</v>
       </c>
       <c r="C137" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D137" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D137" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2941,13 +2941,13 @@
         <v>77</v>
       </c>
       <c r="B138" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C138" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2972,7 +2972,7 @@
         <v>180</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>181</v>
@@ -2986,7 +2986,7 @@
         <v>180</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>128</v>
@@ -3028,7 +3028,7 @@
         <v>180</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D144" s="0" t="s">
         <v>27</v>
@@ -3056,10 +3056,10 @@
         <v>183</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3067,13 +3067,13 @@
         <v>77</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3084,10 +3084,10 @@
         <v>34</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3098,10 +3098,10 @@
         <v>35</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3112,10 +3112,10 @@
         <v>36</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3126,10 +3126,10 @@
         <v>37</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3140,10 +3140,10 @@
         <v>38</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3154,10 +3154,10 @@
         <v>39</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3168,10 +3168,10 @@
         <v>40</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3182,10 +3182,10 @@
         <v>41</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3196,10 +3196,10 @@
         <v>42</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3210,10 +3210,10 @@
         <v>43</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3224,10 +3224,10 @@
         <v>44</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3238,10 +3238,10 @@
         <v>45</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3252,10 +3252,10 @@
         <v>46</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3266,10 +3266,10 @@
         <v>47</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3280,10 +3280,10 @@
         <v>48</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3294,10 +3294,10 @@
         <v>49</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3308,10 +3308,10 @@
         <v>50</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3322,10 +3322,10 @@
         <v>51</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3336,10 +3336,10 @@
         <v>52</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -3350,10 +3350,10 @@
         <v>53</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3364,10 +3364,10 @@
         <v>54</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3378,10 +3378,10 @@
         <v>55</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3392,10 +3392,10 @@
         <v>56</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3406,10 +3406,10 @@
         <v>57</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -3420,10 +3420,10 @@
         <v>58</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3434,10 +3434,10 @@
         <v>59</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3448,10 +3448,10 @@
         <v>60</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3459,10 +3459,10 @@
         <v>77</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>184</v>
@@ -3473,7 +3473,7 @@
         <v>77</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C176" s="0" t="s">
         <v>63</v>
@@ -3487,13 +3487,13 @@
         <v>77</v>
       </c>
       <c r="B177" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C177" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C177" s="0" t="s">
+      <c r="D177" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D177" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3501,7 +3501,7 @@
         <v>77</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C178" s="0" t="s">
         <v>68</v>
@@ -3515,13 +3515,13 @@
         <v>77</v>
       </c>
       <c r="B179" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C179" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C179" s="0" t="s">
+      <c r="D179" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D179" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3529,7 +3529,7 @@
         <v>77</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C180" s="0" t="s">
         <v>73</v>
@@ -3543,7 +3543,7 @@
         <v>77</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C181" s="0" t="s">
         <v>75</v>
@@ -3588,10 +3588,10 @@
         <v>189</v>
       </c>
       <c r="C184" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D184" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D184" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3599,13 +3599,13 @@
         <v>185</v>
       </c>
       <c r="B185" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C185" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C185" s="0" t="s">
+      <c r="D185" s="0" t="s">
         <v>191</v>
-      </c>
-      <c r="D185" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3616,10 +3616,10 @@
         <v>193</v>
       </c>
       <c r="C186" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D186" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D186" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3627,13 +3627,13 @@
         <v>185</v>
       </c>
       <c r="B187" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C187" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C187" s="0" t="s">
+      <c r="D187" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="D187" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3641,7 +3641,7 @@
         <v>185</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C188" s="0" t="s">
         <v>197</v>
@@ -3655,7 +3655,7 @@
         <v>185</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C189" s="0" t="s">
         <v>199</v>
@@ -3669,13 +3669,13 @@
         <v>185</v>
       </c>
       <c r="B190" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D190" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="C190" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D190" s="0" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3683,7 +3683,7 @@
         <v>185</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C191" s="0" t="s">
         <v>107</v>
@@ -3697,7 +3697,7 @@
         <v>185</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C192" s="0" t="s">
         <v>109</v>
@@ -3711,10 +3711,10 @@
         <v>185</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>111</v>
@@ -3725,7 +3725,7 @@
         <v>185</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C194" s="0" t="s">
         <v>17</v>
@@ -3739,7 +3739,7 @@
         <v>185</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C195" s="0" t="s">
         <v>113</v>
@@ -3753,13 +3753,13 @@
         <v>185</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3767,13 +3767,13 @@
         <v>185</v>
       </c>
       <c r="B197" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C197" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C197" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="D197" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3784,10 +3784,10 @@
         <v>34</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3798,10 +3798,10 @@
         <v>35</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3812,10 +3812,10 @@
         <v>36</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3826,10 +3826,10 @@
         <v>37</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3840,10 +3840,10 @@
         <v>38</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3854,10 +3854,10 @@
         <v>39</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3868,10 +3868,10 @@
         <v>40</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3882,10 +3882,10 @@
         <v>41</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3896,10 +3896,10 @@
         <v>42</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3910,10 +3910,10 @@
         <v>43</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3924,10 +3924,10 @@
         <v>44</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3938,10 +3938,10 @@
         <v>45</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3952,10 +3952,10 @@
         <v>46</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3966,10 +3966,10 @@
         <v>47</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3980,10 +3980,10 @@
         <v>48</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3994,10 +3994,10 @@
         <v>49</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4008,10 +4008,10 @@
         <v>50</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4022,10 +4022,10 @@
         <v>51</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4036,10 +4036,10 @@
         <v>52</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4050,10 +4050,10 @@
         <v>53</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4064,10 +4064,10 @@
         <v>54</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4078,10 +4078,10 @@
         <v>55</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4092,10 +4092,10 @@
         <v>56</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4106,10 +4106,10 @@
         <v>57</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -4120,10 +4120,10 @@
         <v>58</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -4134,10 +4134,10 @@
         <v>59</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -4148,10 +4148,10 @@
         <v>60</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -4159,10 +4159,10 @@
         <v>185</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>203</v>
@@ -4173,7 +4173,7 @@
         <v>185</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>63</v>
@@ -4187,13 +4187,13 @@
         <v>185</v>
       </c>
       <c r="B227" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C227" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C227" s="0" t="s">
+      <c r="D227" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D227" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -4201,7 +4201,7 @@
         <v>185</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>68</v>
@@ -4215,13 +4215,13 @@
         <v>185</v>
       </c>
       <c r="B229" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C229" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C229" s="0" t="s">
+      <c r="D229" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D229" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -4229,7 +4229,7 @@
         <v>185</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>73</v>
@@ -4243,7 +4243,7 @@
         <v>185</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>75</v>
@@ -4257,7 +4257,7 @@
         <v>204</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>205</v>
@@ -4271,7 +4271,7 @@
         <v>204</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>207</v>
@@ -4285,7 +4285,7 @@
         <v>204</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>209</v>
@@ -4302,10 +4302,10 @@
         <v>211</v>
       </c>
       <c r="C235" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D235" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D235" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -4316,10 +4316,10 @@
         <v>212</v>
       </c>
       <c r="C236" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D236" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D236" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -4344,7 +4344,7 @@
         <v>212</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D238" s="0" t="s">
         <v>213</v>
@@ -4372,10 +4372,10 @@
         <v>216</v>
       </c>
       <c r="C240" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D240" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D240" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -4386,10 +4386,10 @@
         <v>217</v>
       </c>
       <c r="C241" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D241" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D241" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -4400,7 +4400,7 @@
         <v>217</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D242" s="0" t="s">
         <v>218</v>
@@ -4456,10 +4456,10 @@
         <v>220</v>
       </c>
       <c r="C246" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D246" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D246" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -4498,10 +4498,10 @@
         <v>221</v>
       </c>
       <c r="C249" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D249" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D249" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -4540,10 +4540,10 @@
         <v>222</v>
       </c>
       <c r="C252" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D252" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D252" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -4621,13 +4621,13 @@
         <v>204</v>
       </c>
       <c r="B258" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C258" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D258" s="0" t="s">
         <v>225</v>
-      </c>
-      <c r="C258" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D258" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4635,7 +4635,7 @@
         <v>204</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C259" s="0" t="s">
         <v>107</v>
@@ -4649,7 +4649,7 @@
         <v>204</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C260" s="0" t="s">
         <v>109</v>
@@ -4663,10 +4663,10 @@
         <v>204</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D261" s="0" t="s">
         <v>228</v>
@@ -4677,7 +4677,7 @@
         <v>204</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C262" s="0" t="s">
         <v>115</v>
@@ -4691,13 +4691,13 @@
         <v>204</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C263" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D263" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D263" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4705,7 +4705,7 @@
         <v>204</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C264" s="0" t="s">
         <v>17</v>
@@ -4719,7 +4719,7 @@
         <v>204</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C265" s="0" t="s">
         <v>113</v>
@@ -4733,7 +4733,7 @@
         <v>204</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>231</v>
@@ -4747,7 +4747,7 @@
         <v>204</v>
       </c>
       <c r="B267" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C267" s="0" t="s">
         <v>233</v>
@@ -4764,10 +4764,10 @@
         <v>235</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D268" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4775,13 +4775,13 @@
         <v>204</v>
       </c>
       <c r="B269" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C269" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D269" s="0" t="s">
         <v>236</v>
-      </c>
-      <c r="C269" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D269" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4789,7 +4789,7 @@
         <v>204</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C270" s="0" t="s">
         <v>115</v>
@@ -4803,13 +4803,13 @@
         <v>204</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D271" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4820,10 +4820,10 @@
         <v>34</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D272" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4834,10 +4834,10 @@
         <v>35</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4848,10 +4848,10 @@
         <v>36</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D274" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4862,10 +4862,10 @@
         <v>37</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4876,10 +4876,10 @@
         <v>38</v>
       </c>
       <c r="C276" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D276" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4890,10 +4890,10 @@
         <v>39</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D277" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4904,10 +4904,10 @@
         <v>40</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4918,10 +4918,10 @@
         <v>41</v>
       </c>
       <c r="C279" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4932,10 +4932,10 @@
         <v>42</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D280" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4946,10 +4946,10 @@
         <v>43</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D281" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4960,10 +4960,10 @@
         <v>44</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D282" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4974,10 +4974,10 @@
         <v>45</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D283" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4988,10 +4988,10 @@
         <v>46</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D284" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5002,10 +5002,10 @@
         <v>47</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D285" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5016,10 +5016,10 @@
         <v>48</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5030,10 +5030,10 @@
         <v>49</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5044,10 +5044,10 @@
         <v>50</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D288" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5058,10 +5058,10 @@
         <v>51</v>
       </c>
       <c r="C289" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D289" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5072,10 +5072,10 @@
         <v>52</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D290" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5086,10 +5086,10 @@
         <v>53</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5100,10 +5100,10 @@
         <v>54</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D292" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -5114,10 +5114,10 @@
         <v>55</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D293" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -5128,10 +5128,10 @@
         <v>56</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -5142,10 +5142,10 @@
         <v>57</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D295" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -5156,10 +5156,10 @@
         <v>58</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -5170,10 +5170,10 @@
         <v>59</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -5184,10 +5184,10 @@
         <v>60</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -5195,10 +5195,10 @@
         <v>204</v>
       </c>
       <c r="B299" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D299" s="0" t="s">
         <v>238</v>
@@ -5209,7 +5209,7 @@
         <v>204</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C300" s="0" t="s">
         <v>63</v>
@@ -5223,13 +5223,13 @@
         <v>204</v>
       </c>
       <c r="B301" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C301" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C301" s="0" t="s">
+      <c r="D301" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D301" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -5237,7 +5237,7 @@
         <v>204</v>
       </c>
       <c r="B302" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C302" s="0" t="s">
         <v>68</v>
@@ -5251,13 +5251,13 @@
         <v>204</v>
       </c>
       <c r="B303" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C303" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C303" s="0" t="s">
+      <c r="D303" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D303" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -5265,7 +5265,7 @@
         <v>204</v>
       </c>
       <c r="B304" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C304" s="0" t="s">
         <v>73</v>
@@ -5279,7 +5279,7 @@
         <v>204</v>
       </c>
       <c r="B305" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C305" s="0" t="s">
         <v>75</v>
@@ -5293,7 +5293,7 @@
         <v>239</v>
       </c>
       <c r="B306" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C306" s="0" t="s">
         <v>240</v>
@@ -5310,10 +5310,10 @@
         <v>220</v>
       </c>
       <c r="C307" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D307" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D307" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -5394,7 +5394,7 @@
         <v>242</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D313" s="0" t="s">
         <v>111</v>
@@ -5419,13 +5419,13 @@
         <v>239</v>
       </c>
       <c r="B315" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C315" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="C315" s="0" t="s">
+      <c r="D315" s="0" t="s">
         <v>244</v>
-      </c>
-      <c r="D315" s="0" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -5436,10 +5436,10 @@
         <v>246</v>
       </c>
       <c r="C316" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D316" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D316" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -5464,10 +5464,10 @@
         <v>247</v>
       </c>
       <c r="C318" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D318" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D318" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -5520,7 +5520,7 @@
         <v>248</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D322" s="0" t="s">
         <v>111</v>
@@ -5562,7 +5562,7 @@
         <v>248</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D325" s="0" t="s">
         <v>249</v>
@@ -5573,13 +5573,13 @@
         <v>239</v>
       </c>
       <c r="B326" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D326" s="0" t="s">
         <v>250</v>
-      </c>
-      <c r="C326" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D326" s="0" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -5587,13 +5587,13 @@
         <v>239</v>
       </c>
       <c r="B327" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5601,13 +5601,13 @@
         <v>239</v>
       </c>
       <c r="B328" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D328" s="0" t="s">
         <v>252</v>
-      </c>
-      <c r="C328" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D328" s="0" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5615,13 +5615,13 @@
         <v>239</v>
       </c>
       <c r="B329" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D329" s="0" t="s">
         <v>254</v>
-      </c>
-      <c r="C329" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D329" s="0" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -5660,7 +5660,7 @@
         <v>256</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D332" s="0" t="s">
         <v>111</v>
@@ -5716,7 +5716,7 @@
         <v>256</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D336" s="0" t="s">
         <v>257</v>
@@ -5730,10 +5730,10 @@
         <v>258</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5744,10 +5744,10 @@
         <v>259</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5758,10 +5758,10 @@
         <v>260</v>
       </c>
       <c r="C339" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D339" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D339" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5772,10 +5772,10 @@
         <v>261</v>
       </c>
       <c r="C340" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D340" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D340" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5783,13 +5783,13 @@
         <v>239</v>
       </c>
       <c r="B341" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D341" s="0" t="s">
         <v>262</v>
-      </c>
-      <c r="C341" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D341" s="0" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5797,13 +5797,13 @@
         <v>239</v>
       </c>
       <c r="B342" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D342" s="0" t="s">
         <v>264</v>
-      </c>
-      <c r="C342" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D342" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5811,7 +5811,7 @@
         <v>239</v>
       </c>
       <c r="B343" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C343" s="0" t="s">
         <v>107</v>
@@ -5825,7 +5825,7 @@
         <v>239</v>
       </c>
       <c r="B344" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C344" s="0" t="s">
         <v>109</v>
@@ -5839,7 +5839,7 @@
         <v>239</v>
       </c>
       <c r="B345" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C345" s="0" t="s">
         <v>115</v>
@@ -5853,10 +5853,10 @@
         <v>239</v>
       </c>
       <c r="B346" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D346" s="0" t="s">
         <v>111</v>
@@ -5867,7 +5867,7 @@
         <v>239</v>
       </c>
       <c r="B347" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C347" s="0" t="s">
         <v>17</v>
@@ -5881,7 +5881,7 @@
         <v>239</v>
       </c>
       <c r="B348" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C348" s="0" t="s">
         <v>113</v>
@@ -5898,10 +5898,10 @@
         <v>266</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5912,10 +5912,10 @@
         <v>267</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5926,10 +5926,10 @@
         <v>268</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5940,10 +5940,10 @@
         <v>269</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5951,13 +5951,13 @@
         <v>239</v>
       </c>
       <c r="B353" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5968,10 +5968,10 @@
         <v>34</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5982,10 +5982,10 @@
         <v>35</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5996,10 +5996,10 @@
         <v>36</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6010,10 +6010,10 @@
         <v>37</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6024,10 +6024,10 @@
         <v>38</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6038,10 +6038,10 @@
         <v>39</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6052,10 +6052,10 @@
         <v>40</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6066,10 +6066,10 @@
         <v>41</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6080,10 +6080,10 @@
         <v>42</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6094,10 +6094,10 @@
         <v>43</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -6108,10 +6108,10 @@
         <v>44</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -6122,10 +6122,10 @@
         <v>45</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -6136,10 +6136,10 @@
         <v>46</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -6150,10 +6150,10 @@
         <v>47</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -6164,10 +6164,10 @@
         <v>48</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -6178,10 +6178,10 @@
         <v>49</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -6192,10 +6192,10 @@
         <v>50</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -6206,10 +6206,10 @@
         <v>51</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -6220,10 +6220,10 @@
         <v>52</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -6234,10 +6234,10 @@
         <v>53</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D373" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -6248,10 +6248,10 @@
         <v>54</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D374" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -6262,10 +6262,10 @@
         <v>55</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D375" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -6276,10 +6276,10 @@
         <v>56</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D376" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -6290,10 +6290,10 @@
         <v>57</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D377" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -6304,10 +6304,10 @@
         <v>58</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -6318,10 +6318,10 @@
         <v>59</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D379" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -6332,10 +6332,10 @@
         <v>60</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -6343,10 +6343,10 @@
         <v>239</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D381" s="0" t="s">
         <v>270</v>
@@ -6357,7 +6357,7 @@
         <v>239</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C382" s="0" t="s">
         <v>63</v>
@@ -6371,13 +6371,13 @@
         <v>239</v>
       </c>
       <c r="B383" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C383" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C383" s="0" t="s">
+      <c r="D383" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D383" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -6385,7 +6385,7 @@
         <v>239</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C384" s="0" t="s">
         <v>68</v>
@@ -6399,13 +6399,13 @@
         <v>239</v>
       </c>
       <c r="B385" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C385" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C385" s="0" t="s">
+      <c r="D385" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D385" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -6413,7 +6413,7 @@
         <v>239</v>
       </c>
       <c r="B386" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C386" s="0" t="s">
         <v>73</v>
@@ -6427,7 +6427,7 @@
         <v>239</v>
       </c>
       <c r="B387" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C387" s="0" t="s">
         <v>75</v>

</xml_diff>